<commit_message>
PROS-4783 - CCH Integration
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Petroleum PoS 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Petroleum PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Petrol" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,6 +35,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -63,10 +65,10 @@
     <t xml:space="preserve">SAP KPI</t>
   </si>
   <si>
+    <t xml:space="preserve">CCH KPI ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">KPI name Eng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH KPI ID</t>
   </si>
   <si>
     <t xml:space="preserve">KPI name Rus</t>
@@ -1232,11 +1234,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1602,7 +1604,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1680,17 +1681,18 @@
   <dimension ref="A1:AR77"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+      <selection pane="bottomRight" activeCell="G69" activeCellId="0" sqref="G69:G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="14" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
@@ -1718,25 +1720,25 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="6" t="s">
@@ -1748,73 +1750,73 @@
       <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="5" t="s">
         <v>39</v>
       </c>
       <c r="AO1" s="2" t="s">
@@ -1846,10 +1848,10 @@
       <c r="E2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="14"/>
       <c r="H2" s="14" t="s">
         <v>49</v>
       </c>
@@ -1883,12 +1885,12 @@
         <v>50</v>
       </c>
       <c r="AF2" s="15"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
       <c r="AM2" s="17" t="n">
         <v>2</v>
       </c>
@@ -1918,10 +1920,10 @@
       <c r="E3" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="22"/>
       <c r="H3" s="23" t="s">
         <v>54</v>
       </c>
@@ -1971,12 +1973,12 @@
       <c r="AF3" s="27" t="n">
         <v>0.016016</v>
       </c>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
       <c r="AM3" s="17" t="n">
         <v>3</v>
       </c>
@@ -2006,10 +2008,10 @@
       <c r="E4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="22"/>
       <c r="H4" s="23" t="s">
         <v>62</v>
       </c>
@@ -2059,12 +2061,12 @@
       <c r="AF4" s="27" t="n">
         <v>0.016016</v>
       </c>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
       <c r="AM4" s="17" t="n">
         <v>3</v>
       </c>
@@ -2094,10 +2096,10 @@
       <c r="E5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
         <v>64</v>
       </c>
@@ -2182,10 +2184,10 @@
       <c r="E6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="22"/>
       <c r="H6" s="23" t="s">
         <v>66</v>
       </c>
@@ -2235,12 +2237,12 @@
       <c r="AF6" s="27" t="n">
         <v>0.011998</v>
       </c>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
       <c r="AM6" s="17" t="n">
         <v>3</v>
       </c>
@@ -2270,10 +2272,10 @@
       <c r="E7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="22"/>
       <c r="H7" s="23" t="s">
         <v>68</v>
       </c>
@@ -2358,10 +2360,10 @@
       <c r="E8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="22"/>
       <c r="H8" s="23" t="s">
         <v>70</v>
       </c>
@@ -2446,10 +2448,10 @@
       <c r="E9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="22"/>
       <c r="H9" s="23" t="s">
         <v>72</v>
       </c>
@@ -2534,10 +2536,10 @@
       <c r="E10" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="22"/>
       <c r="H10" s="23" t="s">
         <v>74</v>
       </c>
@@ -2622,10 +2624,10 @@
       <c r="E11" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="22"/>
       <c r="H11" s="23" t="s">
         <v>76</v>
       </c>
@@ -2710,10 +2712,10 @@
       <c r="E12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="22"/>
+      <c r="G12" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="22"/>
       <c r="H12" s="23" t="s">
         <v>78</v>
       </c>
@@ -2798,10 +2800,10 @@
       <c r="E13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="22"/>
       <c r="H13" s="23" t="s">
         <v>80</v>
       </c>
@@ -2886,10 +2888,10 @@
       <c r="E14" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="22"/>
       <c r="H14" s="23" t="s">
         <v>82</v>
       </c>
@@ -2974,10 +2976,10 @@
       <c r="E15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="37"/>
       <c r="H15" s="37" t="s">
         <v>85</v>
       </c>
@@ -3046,10 +3048,10 @@
       <c r="E16" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="22"/>
+      <c r="G16" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="22"/>
       <c r="H16" s="23" t="s">
         <v>88</v>
       </c>
@@ -3134,10 +3136,10 @@
       <c r="E17" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="22"/>
+      <c r="G17" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="22"/>
       <c r="H17" s="23" t="s">
         <v>90</v>
       </c>
@@ -3222,10 +3224,10 @@
       <c r="E18" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="22"/>
       <c r="H18" s="23" t="s">
         <v>92</v>
       </c>
@@ -3310,10 +3312,10 @@
       <c r="E19" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="22"/>
       <c r="H19" s="23" t="s">
         <v>94</v>
       </c>
@@ -3398,10 +3400,10 @@
       <c r="E20" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="22"/>
       <c r="H20" s="23" t="s">
         <v>96</v>
       </c>
@@ -3486,10 +3488,10 @@
       <c r="E21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="22"/>
+      <c r="G21" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="22"/>
       <c r="H21" s="23" t="s">
         <v>98</v>
       </c>
@@ -3574,10 +3576,10 @@
       <c r="E22" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="22"/>
       <c r="H22" s="23" t="s">
         <v>100</v>
       </c>
@@ -3662,10 +3664,10 @@
       <c r="E23" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="G23" s="37"/>
       <c r="H23" s="37" t="s">
         <v>102</v>
       </c>
@@ -3734,10 +3736,10 @@
       <c r="E24" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="22"/>
       <c r="H24" s="23" t="s">
         <v>105</v>
       </c>
@@ -3822,10 +3824,10 @@
       <c r="E25" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="22"/>
+      <c r="G25" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="G25" s="22"/>
       <c r="H25" s="23" t="s">
         <v>107</v>
       </c>
@@ -3910,10 +3912,10 @@
       <c r="E26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="22"/>
+      <c r="G26" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="42"/>
       <c r="H26" s="23" t="s">
         <v>109</v>
       </c>
@@ -3998,10 +4000,10 @@
       <c r="E27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="22"/>
+      <c r="G27" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="G27" s="42"/>
       <c r="H27" s="23" t="s">
         <v>111</v>
       </c>
@@ -4086,10 +4088,10 @@
       <c r="E28" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="22"/>
       <c r="H28" s="23" t="s">
         <v>113</v>
       </c>
@@ -4174,10 +4176,10 @@
       <c r="E29" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="22"/>
+      <c r="G29" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="G29" s="22"/>
       <c r="H29" s="23" t="s">
         <v>115</v>
       </c>
@@ -4262,10 +4264,10 @@
       <c r="E30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G30" s="22"/>
       <c r="H30" s="23" t="s">
         <v>117</v>
       </c>
@@ -4350,10 +4352,10 @@
       <c r="E31" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="22"/>
+      <c r="G31" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="22"/>
       <c r="H31" s="23" t="s">
         <v>119</v>
       </c>
@@ -4438,10 +4440,10 @@
       <c r="E32" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="12"/>
+      <c r="G32" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="G32" s="37"/>
       <c r="H32" s="37" t="s">
         <v>121</v>
       </c>
@@ -4510,10 +4512,10 @@
       <c r="E33" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="22"/>
+      <c r="G33" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
         <v>124</v>
       </c>
@@ -4598,10 +4600,10 @@
       <c r="E34" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="22"/>
+      <c r="G34" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="22"/>
       <c r="H34" s="23" t="s">
         <v>126</v>
       </c>
@@ -4686,10 +4688,10 @@
       <c r="E35" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="22"/>
+      <c r="G35" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
         <v>128</v>
       </c>
@@ -4774,10 +4776,10 @@
       <c r="E36" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G36" s="22"/>
       <c r="H36" s="23" t="s">
         <v>130</v>
       </c>
@@ -4862,10 +4864,10 @@
       <c r="E37" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="12"/>
+      <c r="G37" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="G37" s="37"/>
       <c r="H37" s="37" t="s">
         <v>132</v>
       </c>
@@ -4934,10 +4936,10 @@
       <c r="E38" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="22"/>
+      <c r="G38" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G38" s="22"/>
       <c r="H38" s="23" t="s">
         <v>135</v>
       </c>
@@ -5022,10 +5024,10 @@
       <c r="E39" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="22"/>
+      <c r="G39" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="G39" s="22"/>
       <c r="H39" s="23" t="s">
         <v>137</v>
       </c>
@@ -5110,10 +5112,10 @@
       <c r="E40" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="22"/>
+      <c r="G40" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G40" s="22"/>
       <c r="H40" s="23" t="s">
         <v>139</v>
       </c>
@@ -5198,10 +5200,10 @@
       <c r="E41" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="22"/>
+      <c r="G41" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="G41" s="22"/>
       <c r="H41" s="23" t="s">
         <v>141</v>
       </c>
@@ -5286,10 +5288,10 @@
       <c r="E42" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="F42" s="44" t="s">
+      <c r="F42" s="43"/>
+      <c r="G42" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="G42" s="44"/>
       <c r="H42" s="44" t="s">
         <v>144</v>
       </c>
@@ -5380,10 +5382,10 @@
       <c r="E43" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="F43" s="44" t="s">
+      <c r="F43" s="43"/>
+      <c r="G43" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="G43" s="44"/>
       <c r="H43" s="44" t="s">
         <v>155</v>
       </c>
@@ -5474,10 +5476,10 @@
       <c r="E44" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="F44" s="44" t="s">
+      <c r="F44" s="43"/>
+      <c r="G44" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="G44" s="44"/>
       <c r="H44" s="44" t="s">
         <v>159</v>
       </c>
@@ -5568,10 +5570,10 @@
       <c r="E45" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="F45" s="44" t="s">
+      <c r="F45" s="43"/>
+      <c r="G45" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="G45" s="44"/>
       <c r="H45" s="44" t="s">
         <v>163</v>
       </c>
@@ -5662,10 +5664,10 @@
       <c r="E46" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="52"/>
+      <c r="G46" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="G46" s="9"/>
       <c r="H46" s="9" t="s">
         <v>167</v>
       </c>
@@ -5742,10 +5744,10 @@
       <c r="E47" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="52"/>
+      <c r="G47" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G47" s="9"/>
       <c r="H47" s="9" t="s">
         <v>171</v>
       </c>
@@ -5830,10 +5832,10 @@
       <c r="E48" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="52"/>
+      <c r="G48" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G48" s="9"/>
       <c r="H48" s="9" t="s">
         <v>177</v>
       </c>
@@ -5912,10 +5914,10 @@
       <c r="E49" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="52"/>
+      <c r="G49" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="G49" s="9"/>
       <c r="H49" s="9" t="s">
         <v>182</v>
       </c>
@@ -6002,10 +6004,10 @@
       <c r="E50" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="52"/>
+      <c r="G50" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="G50" s="9"/>
       <c r="H50" s="9" t="s">
         <v>186</v>
       </c>
@@ -6088,10 +6090,10 @@
       <c r="E51" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F51" s="44" t="s">
+      <c r="F51" s="43"/>
+      <c r="G51" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="G51" s="44"/>
       <c r="H51" s="9" t="s">
         <v>192</v>
       </c>
@@ -6165,10 +6167,10 @@
       <c r="E52" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F52" s="61" t="s">
+      <c r="F52" s="43"/>
+      <c r="G52" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="G52" s="61"/>
       <c r="H52" s="44" t="s">
         <v>197</v>
       </c>
@@ -6251,10 +6253,10 @@
       <c r="E53" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F53" s="44" t="s">
+      <c r="F53" s="43"/>
+      <c r="G53" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="G53" s="44"/>
       <c r="H53" s="44" t="s">
         <v>204</v>
       </c>
@@ -6335,10 +6337,10 @@
       <c r="E54" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="F54" s="44" t="s">
+      <c r="F54" s="43"/>
+      <c r="G54" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="G54" s="44"/>
       <c r="H54" s="64" t="s">
         <v>209</v>
       </c>
@@ -6423,10 +6425,10 @@
       <c r="E55" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="43"/>
+      <c r="G55" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="G55" s="9"/>
       <c r="H55" s="9" t="s">
         <v>217</v>
       </c>
@@ -6507,10 +6509,10 @@
       <c r="E56" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="43"/>
+      <c r="G56" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="G56" s="9"/>
       <c r="H56" s="9" t="s">
         <v>222</v>
       </c>
@@ -6593,10 +6595,10 @@
       <c r="E57" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="43"/>
+      <c r="G57" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="G57" s="9"/>
       <c r="H57" s="9" t="s">
         <v>226</v>
       </c>
@@ -6685,10 +6687,10 @@
       <c r="E58" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="43"/>
+      <c r="G58" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
         <v>228</v>
       </c>
@@ -6773,10 +6775,10 @@
       <c r="E59" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="43"/>
+      <c r="G59" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="G59" s="9"/>
       <c r="H59" s="9" t="s">
         <v>230</v>
       </c>
@@ -6863,10 +6865,10 @@
       <c r="E60" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="43"/>
+      <c r="G60" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="G60" s="9"/>
       <c r="H60" s="9" t="s">
         <v>235</v>
       </c>
@@ -6947,10 +6949,10 @@
       <c r="E61" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="43"/>
+      <c r="G61" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="G61" s="9"/>
       <c r="H61" s="9" t="s">
         <v>238</v>
       </c>
@@ -7031,10 +7033,10 @@
       <c r="E62" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="43"/>
+      <c r="G62" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="G62" s="9"/>
       <c r="H62" s="9" t="s">
         <v>241</v>
       </c>
@@ -7123,10 +7125,10 @@
       <c r="E63" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="43"/>
+      <c r="G63" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="G63" s="9"/>
       <c r="H63" s="9" t="s">
         <v>245</v>
       </c>
@@ -7213,10 +7215,10 @@
       <c r="E64" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="43"/>
+      <c r="G64" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G64" s="9"/>
       <c r="H64" s="9" t="s">
         <v>248</v>
       </c>
@@ -7299,10 +7301,10 @@
       <c r="E65" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="F65" s="44" t="s">
+      <c r="F65" s="43"/>
+      <c r="G65" s="44" t="s">
         <v>253</v>
       </c>
-      <c r="G65" s="44"/>
       <c r="H65" s="44" t="s">
         <v>254</v>
       </c>
@@ -7393,10 +7395,10 @@
       <c r="E66" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="F66" s="44" t="s">
+      <c r="F66" s="43"/>
+      <c r="G66" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="G66" s="44"/>
       <c r="H66" s="44" t="s">
         <v>260</v>
       </c>
@@ -7487,10 +7489,10 @@
       <c r="E67" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="F67" s="44" t="s">
+      <c r="F67" s="43"/>
+      <c r="G67" s="44" t="s">
         <v>262</v>
       </c>
-      <c r="G67" s="44"/>
       <c r="H67" s="44" t="s">
         <v>263</v>
       </c>
@@ -7581,10 +7583,10 @@
       <c r="E68" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="F68" s="44" t="s">
+      <c r="F68" s="43"/>
+      <c r="G68" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="G68" s="44"/>
       <c r="H68" s="44" t="s">
         <v>266</v>
       </c>
@@ -8315,7 +8317,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AQ69"/>
-  <conditionalFormatting sqref="F3:G14">
+  <conditionalFormatting sqref="G3:G14">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -8325,7 +8327,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:G22">
+  <conditionalFormatting sqref="G16:G22">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -8335,7 +8337,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:G29">
+  <conditionalFormatting sqref="G29">
     <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -8345,7 +8347,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33:G36">
+  <conditionalFormatting sqref="G33:G36">
     <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -8355,7 +8357,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:G41">
+  <conditionalFormatting sqref="G38:G41">
     <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -8384,7 +8386,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G69:G77 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8421,7 +8423,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G69:G77 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8434,7 +8436,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="89" t="s">
         <v>7</v>

</xml_diff>